<commit_message>
Making progress on alpha/beta/gamma div but not quite there yet. All plant specimens entered.
</commit_message>
<xml_diff>
--- a/data/Specimens.xlsx
+++ b/data/Specimens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopheradlam/Desktop/Davis/R/GitHub Repos/Fire_mosaics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D1863E-E748-D74B-A2DE-0BC58344E534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D2BBF0-7995-244C-983F-E08A1BAD85DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="2120" windowWidth="27640" windowHeight="16540" xr2:uid="{771E37EE-3B7E-2E49-8FBC-FE3138B75EAD}"/>
+    <workbookView xWindow="660" yWindow="1920" windowWidth="27640" windowHeight="16540" xr2:uid="{771E37EE-3B7E-2E49-8FBC-FE3138B75EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="162">
   <si>
     <t>number</t>
   </si>
@@ -123,24 +123,15 @@
     <t>Triteleia peduncularis</t>
   </si>
   <si>
-    <t>not the best quality because it was already senescing, but interesting because not really within range?</t>
-  </si>
-  <si>
     <t>Allium acuminatum</t>
   </si>
   <si>
     <t>Cryptantha affinis</t>
   </si>
   <si>
-    <t>note asymetrical scar on nutlet</t>
-  </si>
-  <si>
     <t>check agoseris grandiflora vs retrorsa in herbarium</t>
   </si>
   <si>
-    <t>What I was calling AGGR is acutally AGRE, and what I was calling AGHE is actually AGGR</t>
-  </si>
-  <si>
     <t xml:space="preserve">Penstemon speciosus </t>
   </si>
   <si>
@@ -198,6 +189,9 @@
     <t>If I chose "nutlets adaxially flat" I get C torreyana; if I chose "nutlets adaxially round"/ "stems unbranched", I get C. dissita.</t>
   </si>
   <si>
+    <t>Iris macrosiphon</t>
+  </si>
+  <si>
     <t>Iris tenuissima</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t>Acmispon brachycarpum</t>
   </si>
   <si>
-    <t>OK specimen but small</t>
-  </si>
-  <si>
     <t>Cirsium cymosum</t>
   </si>
   <si>
@@ -439,13 +430,100 @@
   </si>
   <si>
     <t>Perideridia sp.</t>
+  </si>
+  <si>
+    <t>What I was calling AGGR is acutally AGRE, and what I was calling AGHI is actually AGGR</t>
+  </si>
+  <si>
+    <t>site 254 I think, but not recorded</t>
+  </si>
+  <si>
+    <t>not the best quality because it was already senescing, but interesting because not really within range? Take another look to make sure it doesn't match TRCR</t>
+  </si>
+  <si>
+    <t>note asymetrical scar on nutlet; misID as CRRI…. Change all CRRI?</t>
+  </si>
+  <si>
+    <t>check paper survey that there wasn't a separate COGR and COPA</t>
+  </si>
+  <si>
+    <t>OK specimen but small. Check site number</t>
+  </si>
+  <si>
+    <t>Ligusticum californicum</t>
+  </si>
+  <si>
+    <t>Maybe replace all IRTE with IRMA? Check stigmas on 225. Are they triangular or rounded?</t>
+  </si>
+  <si>
+    <t>Festuca occidentalis</t>
+  </si>
+  <si>
+    <t>Pretty sure but could check using grass ID</t>
+  </si>
+  <si>
+    <t>Monardella odoratissima var. glauca</t>
+  </si>
+  <si>
+    <t>Bromus</t>
+  </si>
+  <si>
+    <t>use grass ID; looks non-native</t>
+  </si>
+  <si>
+    <t>Clarkia amoena var huntiana</t>
+  </si>
+  <si>
+    <t>GRASS?</t>
+  </si>
+  <si>
+    <t>Osmorhiza berteroi</t>
+  </si>
+  <si>
+    <t>Stachys rigida var. rigida</t>
+  </si>
+  <si>
+    <t>Lomatium</t>
+  </si>
+  <si>
+    <t>L. macrocarpum? No seed/flowers</t>
+  </si>
+  <si>
+    <t>Castilleja</t>
+  </si>
+  <si>
+    <t>Possibly C. attenuata; loose fitting, netted seed. Corrola +/- glabrous, not pouched</t>
+  </si>
+  <si>
+    <t>also check paper: was there really also COGR?</t>
+  </si>
+  <si>
+    <t>"LIMEGREEN"</t>
+  </si>
+  <si>
+    <t>check paper…. Was I recording PYAP when I meant MOHY?</t>
+  </si>
+  <si>
+    <t>Galium parisiense</t>
+  </si>
+  <si>
+    <t>Hossakia crassicaulis</t>
+  </si>
+  <si>
+    <t>Eurybia radulina</t>
+  </si>
+  <si>
+    <t>Lupinus andersonii</t>
+  </si>
+  <si>
+    <t>Centaurea melitensis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,6 +534,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,9 +567,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C579CD91-7B9F-7741-8D74-DA0138DC153E}">
-  <dimension ref="A1:O87"/>
+  <dimension ref="A1:O113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,16 +924,16 @@
       <c r="A2">
         <v>201</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>263</v>
       </c>
       <c r="J2" t="s">
@@ -888,6 +976,9 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
+      <c r="F4" t="s">
+        <v>134</v>
+      </c>
       <c r="J4" t="s">
         <v>9</v>
       </c>
@@ -895,7 +986,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -915,10 +1006,10 @@
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -935,10 +1026,10 @@
         <v>258</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -979,16 +1070,17 @@
       <c r="A9">
         <v>208</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>251</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1009,21 +1101,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>210</v>
       </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>246</v>
       </c>
-      <c r="F11" t="s">
-        <v>30</v>
+      <c r="F11" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1034,253 +1127,253 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>212</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13">
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="3">
         <v>245</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>213</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>214</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>213</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>214</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" s="3">
+        <v>237</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>215</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>216</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E15">
+      <c r="E17" s="3">
         <v>237</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>215</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>217</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="3">
+        <v>202</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>218</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="3">
+        <v>202</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>219</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="2">
+        <v>202</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>220</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="3">
+        <v>202</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>221</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2">
+        <v>209</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>222</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="3">
+        <v>209</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>223</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>224</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>225</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>216</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17">
-        <v>237</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>217</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18">
-        <v>202</v>
-      </c>
-      <c r="F18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>218</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19">
-        <v>202</v>
-      </c>
-      <c r="F19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>219</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20">
-        <v>202</v>
-      </c>
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>220</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21">
-        <v>202</v>
-      </c>
-      <c r="F21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>221</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22">
+      <c r="D26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="3">
         <v>209</v>
       </c>
-      <c r="F22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>222</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23">
+      <c r="F26" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>226</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="3">
         <v>209</v>
       </c>
-      <c r="F23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>223</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>224</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>225</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26">
-        <v>209</v>
-      </c>
-      <c r="F26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>226</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>227</v>
       </c>
@@ -1289,47 +1382,50 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" s="1">
         <v>204</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>228</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="3">
+        <v>209</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>229</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>228</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E30" s="3">
+        <v>209</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E29">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>229</v>
-      </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30">
-        <v>209</v>
-      </c>
-      <c r="F30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>230</v>
       </c>
@@ -1338,199 +1434,199 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E31" s="1">
         <v>207</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>231</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>232</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>231</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E33" s="3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>233</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E32">
+      <c r="E34" s="3">
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>232</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>234</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="3">
+        <v>207</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>235</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D33" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>233</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>234</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="D36" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E35">
-        <v>207</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E36" s="3">
+        <v>204</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>236</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>235</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="E37" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>237</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="3">
+        <v>204</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>238</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E36">
+      <c r="E39" s="3">
         <v>204</v>
       </c>
-      <c r="F36" t="s">
-        <v>71</v>
-      </c>
-      <c r="G36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>236</v>
-      </c>
-      <c r="B37" t="s">
+    </row>
+    <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>238</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>239</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>237</v>
-      </c>
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="D41" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E38">
-        <v>204</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E41" s="3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>240</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="2">
+        <v>266</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>241</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="3">
+        <v>265</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>238</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>238</v>
-      </c>
-      <c r="B40" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>239</v>
-      </c>
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>240</v>
-      </c>
-      <c r="B42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" t="s">
-        <v>43</v>
-      </c>
-      <c r="E42">
-        <v>266</v>
-      </c>
-      <c r="F42" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>241</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" t="s">
-        <v>78</v>
-      </c>
-      <c r="E43">
-        <v>265</v>
-      </c>
-      <c r="F43" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1547,7 +1643,7 @@
         <v>266</v>
       </c>
       <c r="F44" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1564,7 +1660,7 @@
         <v>238</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1575,13 +1671,13 @@
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E46">
         <v>228</v>
       </c>
       <c r="F46" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1592,13 +1688,13 @@
         <v>28</v>
       </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E47">
         <v>228</v>
       </c>
       <c r="F47" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1609,13 +1705,13 @@
         <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E48">
         <v>226</v>
       </c>
       <c r="F48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1626,13 +1722,13 @@
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E49">
         <v>228</v>
       </c>
       <c r="F49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1643,13 +1739,13 @@
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E50">
         <v>226</v>
       </c>
       <c r="F50" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1660,7 +1756,7 @@
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E51">
         <v>226</v>
@@ -1674,7 +1770,7 @@
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E52">
         <v>206</v>
@@ -1689,13 +1785,16 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E53" s="1">
         <v>206</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1706,13 +1805,13 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E54">
         <v>208</v>
       </c>
       <c r="F54" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1723,26 +1822,27 @@
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E55">
         <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>254</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D56" t="s">
-        <v>99</v>
-      </c>
-      <c r="E56">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="2">
         <v>207</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1754,7 +1854,7 @@
         <v>28</v>
       </c>
       <c r="D57" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E57">
         <v>213</v>
@@ -1768,7 +1868,7 @@
         <v>28</v>
       </c>
       <c r="D58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E58">
         <v>215</v>
@@ -1782,13 +1882,13 @@
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E59">
         <v>213</v>
       </c>
       <c r="F59" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1799,7 +1899,7 @@
         <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E60">
         <v>213</v>
@@ -1813,13 +1913,13 @@
         <v>11</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E61">
         <v>213</v>
       </c>
       <c r="F61" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1830,7 +1930,7 @@
         <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E62">
         <v>214</v>
@@ -1847,13 +1947,13 @@
         <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>107</v>
-      </c>
-      <c r="E63">
+        <v>104</v>
+      </c>
+      <c r="E63" s="1">
         <v>221</v>
       </c>
       <c r="G63" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -1864,7 +1964,7 @@
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E64">
         <v>223</v>
@@ -1878,10 +1978,13 @@
         <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E65">
         <v>223</v>
+      </c>
+      <c r="F65" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1892,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E66">
         <v>226</v>
@@ -1906,13 +2009,13 @@
         <v>7</v>
       </c>
       <c r="D67" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E67">
         <v>226</v>
       </c>
       <c r="F67" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -1923,7 +2026,7 @@
         <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E68">
         <v>224</v>
@@ -1937,7 +2040,7 @@
         <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E69">
         <v>224</v>
@@ -1951,7 +2054,7 @@
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E70">
         <v>224</v>
@@ -1965,7 +2068,7 @@
         <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E71">
         <v>224</v>
@@ -1979,13 +2082,13 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E72">
         <v>226</v>
       </c>
       <c r="F72" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -1996,13 +2099,13 @@
         <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E73">
         <v>56</v>
       </c>
       <c r="F73" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2013,7 +2116,7 @@
         <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E74">
         <v>56</v>
@@ -2027,7 +2130,7 @@
         <v>7</v>
       </c>
       <c r="D75" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E75">
         <v>32</v>
@@ -2041,7 +2144,7 @@
         <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E76">
         <v>34</v>
@@ -2055,7 +2158,7 @@
         <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E77">
         <v>32</v>
@@ -2069,13 +2172,13 @@
         <v>9</v>
       </c>
       <c r="D78" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E78" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F78" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2086,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="D79" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E79">
         <v>8</v>
@@ -2100,13 +2203,13 @@
         <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E80">
         <v>7</v>
       </c>
       <c r="F80" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2117,13 +2220,13 @@
         <v>28</v>
       </c>
       <c r="D81" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E81">
         <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2135,13 +2238,13 @@
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E82" s="1">
         <v>7</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2152,7 +2255,7 @@
         <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E83">
         <v>7</v>
@@ -2166,13 +2269,13 @@
         <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E84">
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2183,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E85">
         <v>7</v>
@@ -2197,13 +2300,13 @@
         <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E86">
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2214,10 +2317,398 @@
         <v>11</v>
       </c>
       <c r="D87" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E87">
         <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>286</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>139</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>287</v>
+      </c>
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89">
+        <v>60</v>
+      </c>
+      <c r="F89" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>288</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" t="s">
+        <v>141</v>
+      </c>
+      <c r="E90">
+        <v>54</v>
+      </c>
+      <c r="F90" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>289</v>
+      </c>
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" t="s">
+        <v>141</v>
+      </c>
+      <c r="E91">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>290</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" t="s">
+        <v>143</v>
+      </c>
+      <c r="E92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>291</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" t="s">
+        <v>65</v>
+      </c>
+      <c r="E93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>292</v>
+      </c>
+      <c r="B94" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" t="s">
+        <v>96</v>
+      </c>
+      <c r="E94">
+        <v>5</v>
+      </c>
+      <c r="F94" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>293</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" t="s">
+        <v>144</v>
+      </c>
+      <c r="E95">
+        <v>4</v>
+      </c>
+      <c r="F95" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>294</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>146</v>
+      </c>
+      <c r="E96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>295</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>128</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>296</v>
+      </c>
+      <c r="B98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" t="s">
+        <v>147</v>
+      </c>
+      <c r="E98">
+        <v>6</v>
+      </c>
+      <c r="F98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>297</v>
+      </c>
+      <c r="B99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>49</v>
+      </c>
+      <c r="E99">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>298</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>122</v>
+      </c>
+      <c r="E100">
+        <v>6</v>
+      </c>
+      <c r="F100" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>299</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" t="s">
+        <v>81</v>
+      </c>
+      <c r="E101">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>300</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>148</v>
+      </c>
+      <c r="E102">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>301</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>149</v>
+      </c>
+      <c r="E103">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>302</v>
+      </c>
+      <c r="B104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>150</v>
+      </c>
+      <c r="E104">
+        <v>56</v>
+      </c>
+      <c r="F104" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>303</v>
+      </c>
+      <c r="B105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>38</v>
+      </c>
+      <c r="E105">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>304</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" t="s">
+        <v>152</v>
+      </c>
+      <c r="E106">
+        <v>56</v>
+      </c>
+      <c r="F106" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>305</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E107" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>306</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>307</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E109" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>308</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E110" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
+        <v>309</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E111" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>310</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E112" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>311</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E113" s="2">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many changes, incl. adding .bib, finish lichen data, etc
</commit_message>
<xml_diff>
--- a/data/Specimens.xlsx
+++ b/data/Specimens.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopheradlam/Desktop/Davis/R/GitHub Repos/Fire_mosaics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D2BBF0-7995-244C-983F-E08A1BAD85DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C982EBB4-8222-FB48-A2AD-A4A93707E9FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1920" windowWidth="27640" windowHeight="16540" xr2:uid="{771E37EE-3B7E-2E49-8FBC-FE3138B75EAD}"/>
+    <workbookView xWindow="320" yWindow="4700" windowWidth="27640" windowHeight="16540" xr2:uid="{771E37EE-3B7E-2E49-8FBC-FE3138B75EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="163">
   <si>
     <t>number</t>
   </si>
@@ -105,12 +105,6 @@
     <t>hairy, previously listed as A. heterophylla</t>
   </si>
   <si>
-    <t>grass?</t>
-  </si>
-  <si>
-    <t>use grass ID</t>
-  </si>
-  <si>
     <t>Sidalcea glaucescens</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>misID as gnaphalium</t>
   </si>
   <si>
-    <t>grass</t>
-  </si>
-  <si>
     <t>Madia exigua</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>Cryptantha torreyana</t>
   </si>
   <si>
-    <t>Melica?</t>
-  </si>
-  <si>
     <t xml:space="preserve">unidentified </t>
   </si>
   <si>
@@ -321,9 +309,6 @@
     <t>Stachys rigida</t>
   </si>
   <si>
-    <t>Bromus carinatus?</t>
-  </si>
-  <si>
     <t>Moehringia macrophylla</t>
   </si>
   <si>
@@ -342,9 +327,6 @@
     <t>just dead plant matter</t>
   </si>
   <si>
-    <t>Bromus?</t>
-  </si>
-  <si>
     <t>Acmispon nevadensis</t>
   </si>
   <si>
@@ -474,9 +456,6 @@
     <t>Clarkia amoena var huntiana</t>
   </si>
   <si>
-    <t>GRASS?</t>
-  </si>
-  <si>
     <t>Osmorhiza berteroi</t>
   </si>
   <si>
@@ -498,9 +477,6 @@
     <t>also check paper: was there really also COGR?</t>
   </si>
   <si>
-    <t>"LIMEGREEN"</t>
-  </si>
-  <si>
     <t>check paper…. Was I recording PYAP when I meant MOHY?</t>
   </si>
   <si>
@@ -517,6 +493,33 @@
   </si>
   <si>
     <t>Centaurea melitensis</t>
+  </si>
+  <si>
+    <t>Agrostis stolonifera</t>
+  </si>
+  <si>
+    <t>Stipa stillmanii</t>
+  </si>
+  <si>
+    <t>Melica harfordii</t>
+  </si>
+  <si>
+    <t>Bromus laevipes</t>
+  </si>
+  <si>
+    <t>Bromus orcuttianus</t>
+  </si>
+  <si>
+    <t>"FUZZY", but "LIMEGREEN" also recorded in plot; but also, it's fuzzier than BROR seems to be…</t>
+  </si>
+  <si>
+    <t>Bromus carinatus</t>
+  </si>
+  <si>
+    <t>"FUZZY" now B. sitchensis var carinatus?</t>
+  </si>
+  <si>
+    <t>Bromus sterilis</t>
   </si>
 </sst>
 </file>
@@ -888,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C579CD91-7B9F-7741-8D74-DA0138DC153E}">
   <dimension ref="A1:O113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,7 +980,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J4" t="s">
         <v>9</v>
@@ -986,7 +989,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -1006,10 +1009,10 @@
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1026,10 +1029,10 @@
         <v>258</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1075,14 +1078,12 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>162</v>
       </c>
       <c r="E9" s="2">
         <v>251</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1092,13 +1093,13 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>250</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1110,13 +1111,13 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1">
         <v>246</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1127,7 +1128,7 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>246</v>
@@ -1141,13 +1142,13 @@
         <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" s="3">
         <v>245</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1172,13 +1173,13 @@
         <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3">
         <v>237</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1189,7 +1190,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3">
         <v>237</v>
@@ -1203,13 +1204,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" s="3">
         <v>237</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1217,16 +1218,16 @@
         <v>217</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="3">
         <v>202</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1234,34 +1235,33 @@
         <v>218</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E19" s="3">
         <v>202</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>219</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="3">
         <v>202</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
@@ -1271,30 +1271,28 @@
         <v>7</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E21" s="3">
         <v>202</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>221</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="3">
         <v>209</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1305,13 +1303,13 @@
         <v>11</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E23" s="3">
         <v>209</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1322,7 +1320,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E24" s="3">
         <v>202</v>
@@ -1336,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E25" s="3">
         <v>209</v>
@@ -1350,13 +1348,13 @@
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E26" s="3">
         <v>209</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1367,7 +1365,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E27" s="3">
         <v>209</v>
@@ -1382,13 +1380,13 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E28" s="1">
         <v>204</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1399,13 +1397,13 @@
         <v>7</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E29" s="3">
         <v>209</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1416,13 +1414,13 @@
         <v>7</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E30" s="3">
         <v>209</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1434,13 +1432,13 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E31" s="1">
         <v>207</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1451,7 +1449,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E32" s="3">
         <v>207</v>
@@ -1465,7 +1463,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E33" s="3">
         <v>207</v>
@@ -1479,7 +1477,7 @@
         <v>7</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E34" s="3">
         <v>207</v>
@@ -1493,13 +1491,13 @@
         <v>5</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E35" s="3">
         <v>207</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1510,16 +1508,16 @@
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E36" s="3">
         <v>204</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1530,7 +1528,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E37" s="3">
         <v>204</v>
@@ -1544,13 +1542,13 @@
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E38" s="3">
         <v>204</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1561,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E39" s="3">
         <v>204</v>
@@ -1572,10 +1570,10 @@
         <v>238</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E40" s="3">
         <v>203</v>
@@ -1589,27 +1587,25 @@
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E41" s="3">
         <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="A42" s="3">
         <v>240</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" s="2">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="3">
         <v>266</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1617,16 +1613,16 @@
         <v>241</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E43" s="3">
         <v>265</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1637,13 +1633,13 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E44">
         <v>266</v>
       </c>
       <c r="F44" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1651,16 +1647,16 @@
         <v>243</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E45">
         <v>238</v>
       </c>
       <c r="F45" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1671,13 +1667,13 @@
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E46">
         <v>228</v>
       </c>
       <c r="F46" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1685,16 +1681,16 @@
         <v>245</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E47">
         <v>228</v>
       </c>
       <c r="F47" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1702,16 +1698,16 @@
         <v>246</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E48">
         <v>226</v>
       </c>
       <c r="F48" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1722,13 +1718,13 @@
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E49">
         <v>228</v>
       </c>
       <c r="F49" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1739,13 +1735,13 @@
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E50">
         <v>226</v>
       </c>
       <c r="F50" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1756,7 +1752,7 @@
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E51">
         <v>226</v>
@@ -1770,7 +1766,7 @@
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E52">
         <v>206</v>
@@ -1785,16 +1781,16 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E53" s="1">
         <v>206</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1805,13 +1801,13 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E54">
         <v>208</v>
       </c>
       <c r="F54" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1822,28 +1818,28 @@
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E55">
         <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
+      <c r="A56" s="3">
         <v>254</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="2">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E56" s="3">
         <v>207</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>25</v>
+      <c r="F56" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1851,10 +1847,10 @@
         <v>255</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D57" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E57">
         <v>213</v>
@@ -1865,10 +1861,10 @@
         <v>256</v>
       </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E58">
         <v>215</v>
@@ -1882,13 +1878,13 @@
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E59">
         <v>213</v>
       </c>
       <c r="F59" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1899,7 +1895,7 @@
         <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E60">
         <v>213</v>
@@ -1913,13 +1909,13 @@
         <v>11</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E61">
         <v>213</v>
       </c>
       <c r="F61" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1927,16 +1923,13 @@
         <v>260</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
       <c r="E62">
         <v>214</v>
-      </c>
-      <c r="F62" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -1947,13 +1940,13 @@
         <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E63" s="1">
         <v>221</v>
       </c>
       <c r="G63" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -1964,7 +1957,7 @@
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E64">
         <v>223</v>
@@ -1978,13 +1971,13 @@
         <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
       <c r="E65">
         <v>223</v>
       </c>
       <c r="F65" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1995,7 +1988,7 @@
         <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E66">
         <v>226</v>
@@ -2009,13 +2002,13 @@
         <v>7</v>
       </c>
       <c r="D67" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E67">
         <v>226</v>
       </c>
       <c r="F67" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2026,7 +2019,7 @@
         <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E68">
         <v>224</v>
@@ -2040,7 +2033,7 @@
         <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E69">
         <v>224</v>
@@ -2054,7 +2047,7 @@
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E70">
         <v>224</v>
@@ -2068,7 +2061,7 @@
         <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E71">
         <v>224</v>
@@ -2082,13 +2075,13 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E72">
         <v>226</v>
       </c>
       <c r="F72" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2099,13 +2092,13 @@
         <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E73">
         <v>56</v>
       </c>
       <c r="F73" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2116,7 +2109,7 @@
         <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E74">
         <v>56</v>
@@ -2130,7 +2123,7 @@
         <v>7</v>
       </c>
       <c r="D75" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E75">
         <v>32</v>
@@ -2144,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E76">
         <v>34</v>
@@ -2158,7 +2151,7 @@
         <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E77">
         <v>32</v>
@@ -2172,13 +2165,13 @@
         <v>9</v>
       </c>
       <c r="D78" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E78" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F78" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2189,7 +2182,7 @@
         <v>7</v>
       </c>
       <c r="D79" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E79">
         <v>8</v>
@@ -2203,13 +2196,13 @@
         <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E80">
         <v>7</v>
       </c>
       <c r="F80" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2217,16 +2210,16 @@
         <v>279</v>
       </c>
       <c r="B81" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E81">
         <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2238,13 +2231,13 @@
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E82" s="1">
         <v>7</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2255,7 +2248,7 @@
         <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E83">
         <v>7</v>
@@ -2269,13 +2262,13 @@
         <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E84">
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2286,7 +2279,7 @@
         <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E85">
         <v>7</v>
@@ -2300,13 +2293,13 @@
         <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E86">
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2317,7 +2310,7 @@
         <v>11</v>
       </c>
       <c r="D87" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E87">
         <v>7</v>
@@ -2331,7 +2324,7 @@
         <v>7</v>
       </c>
       <c r="D88" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E88">
         <v>2</v>
@@ -2345,13 +2338,13 @@
         <v>7</v>
       </c>
       <c r="D89" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E89">
         <v>60</v>
       </c>
       <c r="F89" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2362,13 +2355,13 @@
         <v>7</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E90">
         <v>54</v>
       </c>
       <c r="F90" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -2379,7 +2372,7 @@
         <v>7</v>
       </c>
       <c r="D91" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E91">
         <v>54</v>
@@ -2393,7 +2386,7 @@
         <v>7</v>
       </c>
       <c r="D92" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E92">
         <v>5</v>
@@ -2407,7 +2400,7 @@
         <v>7</v>
       </c>
       <c r="D93" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E93">
         <v>5</v>
@@ -2418,16 +2411,13 @@
         <v>292</v>
       </c>
       <c r="B94" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D94" t="s">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="E94">
         <v>5</v>
-      </c>
-      <c r="F94" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2438,13 +2428,13 @@
         <v>11</v>
       </c>
       <c r="D95" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E95">
         <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2455,7 +2445,7 @@
         <v>7</v>
       </c>
       <c r="D96" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E96">
         <v>4</v>
@@ -2469,7 +2459,7 @@
         <v>7</v>
       </c>
       <c r="D97" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E97">
         <v>4</v>
@@ -2480,16 +2470,13 @@
         <v>296</v>
       </c>
       <c r="B98" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D98" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E98">
         <v>6</v>
-      </c>
-      <c r="F98" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -2500,7 +2487,7 @@
         <v>7</v>
       </c>
       <c r="D99" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E99">
         <v>6</v>
@@ -2514,13 +2501,13 @@
         <v>7</v>
       </c>
       <c r="D100" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E100">
         <v>6</v>
       </c>
       <c r="F100" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -2531,7 +2518,7 @@
         <v>7</v>
       </c>
       <c r="D101" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E101">
         <v>6</v>
@@ -2545,7 +2532,7 @@
         <v>7</v>
       </c>
       <c r="D102" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E102">
         <v>6</v>
@@ -2559,7 +2546,7 @@
         <v>7</v>
       </c>
       <c r="D103" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E103">
         <v>6</v>
@@ -2573,13 +2560,13 @@
         <v>9</v>
       </c>
       <c r="D104" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E104">
         <v>56</v>
       </c>
       <c r="F104" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -2590,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="D105" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E105">
         <v>56</v>
@@ -2604,110 +2591,115 @@
         <v>9</v>
       </c>
       <c r="D106" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E106">
         <v>56</v>
       </c>
       <c r="F106" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>305</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E107" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>306</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>307</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E109" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>308</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E110" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>309</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="2">
-        <v>305</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E107" s="2">
+      <c r="E111" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="2">
-        <v>306</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="2">
-        <v>307</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E109" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="2">
-        <v>308</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E110" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="2">
-        <v>309</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E111" s="2">
-        <v>56</v>
-      </c>
-    </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="2">
+      <c r="A112" s="3">
         <v>310</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E112" s="2">
+      <c r="B112" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E112" s="3">
         <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="2">
+      <c r="A113" s="3">
         <v>311</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E113" s="2">
+      <c r="B113" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E113" s="3">
         <v>18</v>
       </c>
     </row>

</xml_diff>